<commit_message>
Change chameleon selection behaviour
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart-\Documents\BoardGameArenaStudio\dale-of-merchants\genmaterial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart-\Documents\BoardGameArenaStudio\dale-of-merchants\misc\genmaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164159E6-E053-46ED-B1D2-8BF769873C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF81FE7-96A7-4B73-A222-7648C4053469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -635,7 +635,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,9 +1008,6 @@
       <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
-        <v>90</v>
-      </c>
       <c r="G16">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Refactor framework for passive abilities
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart-\Documents\BoardGameArenaStudio\dale-of-merchants\misc\genmaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF81FE7-96A7-4B73-A222-7648C4053469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC8EE5-C523-46F4-AF1A-5F89C1F3A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,10 +311,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>has_active</t>
-  </si>
-  <si>
     <t>Prepaid Good</t>
+  </si>
+  <si>
+    <t>has_ability</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -980,7 +980,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Parse die icons in tooltips
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart-\Documents\BoardGameArenaStudio\dale-of-merchants\misc\genmaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AA64A1-6BAD-4E21-8410-CE12247BCE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3371E3D1-C9F6-44A2-BCFF-6F96D6ECCE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1058,15 +1058,6 @@
     <t>Ditch 1 card. Gain 1 COIN.</t>
   </si>
   <si>
-    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2 until you have a different results. Place 1 card from any player's [source] into their [destination].</t>
-  </si>
-  <si>
-    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2. Place a card from any player's [source] into a different player's [destination].</t>
-  </si>
-  <si>
-    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2. Shuffle 2 cards from any player's [source] into a different player's [destination]. Repeat with [destination] and [source] swapped without shuffling.</t>
-  </si>
-  <si>
     <t>When purchased, ditch 0-3 junk used in the purchase.</t>
   </si>
   <si>
@@ -1137,6 +1128,15 @@
   </si>
   <si>
     <t>Draw [DAY 3] [NIGHT 1] cards. Place [DAY 2] [NIGHT 1] cards on top of your deck.</t>
+  </si>
+  <si>
+    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2 until you have a different results. Place 1 card from any player's SOURCE into their DESTINATION.</t>
+  </si>
+  <si>
+    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2. Place a card from any player's SOURCE into a different player's DESTINATION.</t>
+  </si>
+  <si>
+    <t>Roll DIE_PANGOLIN1 and DIE_PANGOLIN2. Shuffle 2 cards from any player's SOURCE into a different player's DESTINATION. Repeat with DESTINATION and SOURCE swapped without shuffling.</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1491,7 @@
   <dimension ref="A1:J169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A137" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+      <selection activeCell="C151" sqref="A1:J169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2076,7 +2076,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>54</v>
@@ -2532,7 +2532,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>54</v>
@@ -2954,7 +2954,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>54</v>
@@ -3638,7 +3638,7 @@
         <v>120</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -3946,7 +3946,7 @@
         <v>174</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4000,7 +4000,7 @@
         <v>176</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>54</v>
@@ -4030,7 +4030,7 @@
         <v>177</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>54</v>
@@ -4060,7 +4060,7 @@
         <v>178</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>54</v>
@@ -4438,7 +4438,7 @@
         <v>191</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>54</v>
@@ -4852,7 +4852,7 @@
         <v>205</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -4938,7 +4938,7 @@
         <v>208</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>54</v>
@@ -5110,7 +5110,7 @@
         <v>240</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>54</v>
@@ -5320,7 +5320,7 @@
         <v>247</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>54</v>
@@ -5588,7 +5588,7 @@
         <v>256</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>54</v>
@@ -5618,7 +5618,7 @@
         <v>257</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>54</v>
@@ -5708,7 +5708,7 @@
         <v>260</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>54</v>
@@ -5738,7 +5738,7 @@
         <v>261</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -5796,7 +5796,7 @@
         <v>263</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>54</v>
@@ -5826,7 +5826,7 @@
         <v>264</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>342</v>
+        <v>366</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>54</v>
@@ -5886,7 +5886,7 @@
         <v>266</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>54</v>
@@ -5916,7 +5916,7 @@
         <v>267</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>54</v>
@@ -5976,7 +5976,7 @@
         <v>269</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>54</v>
@@ -6036,7 +6036,7 @@
         <v>271</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>54</v>
@@ -6122,7 +6122,7 @@
         <v>274</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>54</v>
@@ -6152,7 +6152,7 @@
         <v>275</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>54</v>
@@ -6212,7 +6212,7 @@
         <v>277</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>

</xml_diff>

<commit_message>
Update CT_CUNNINGNEIGHBOUR from Technique to Passive
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="377">
   <si>
     <t>type_id</t>
   </si>
@@ -3277,13 +3277,11 @@
       <c r="C62" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1">
         <v>1.0</v>

</xml_diff>

<commit_message>
Add CT_AVIDFINANCIER and the concept of the "SCHEDULE_COOLDOWN"
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="377">
   <si>
     <t>type_id</t>
   </si>
@@ -1438,7 +1438,7 @@
     <col customWidth="1" min="4" max="4" width="11.29"/>
     <col customWidth="1" min="5" max="5" width="9.86"/>
     <col customWidth="1" min="6" max="6" width="11.43"/>
-    <col customWidth="1" min="7" max="7" width="9.29"/>
+    <col customWidth="1" min="7" max="7" width="15.14"/>
     <col customWidth="1" min="8" max="8" width="6.43"/>
     <col customWidth="1" min="9" max="9" width="10.57"/>
     <col customWidth="1" min="10" max="10" width="14.71"/>
@@ -5298,7 +5298,9 @@
         <v>18</v>
       </c>
       <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
+      <c r="G128" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="H128" s="1">
         <v>1.0</v>
       </c>

</xml_diff>

<commit_message>
Add `'client_spend'` and CT_GREED
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material.xlsx
+++ b/misc/genmaterial/material.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="eT2MBq0ZNOUdV1q1FgyBvVwhpcl16lWyVGJnSyvx6B4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="yCS/AUqO6tbZVXrRq/kgzoxiBgZysP8LVi48y8yfzAc="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="377">
   <si>
     <t>type_id</t>
   </si>
@@ -5324,13 +5324,11 @@
       <c r="C129" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1">
         <v>2.0</v>

</xml_diff>